<commit_message>
Modify database for formula search test, GUI + Latex Viewer + mathml checker for inserting formula test
</commit_message>
<xml_diff>
--- a/search/fsearch/Test_Formulas.xlsx
+++ b/search/fsearch/Test_Formulas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Logarithms</t>
   </si>
   <si>
     <t>Question Source</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>\log_ab</t>
+  </si>
+  <si>
+    <t>\frac{1}{\log_ab}</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>200604003003</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -68,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,28 +366,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latex Viewer + Input + Test data
</commit_message>
<xml_diff>
--- a/search/fsearch/Test_Formulas.xlsx
+++ b/search/fsearch/Test_Formulas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Logarithms</t>
   </si>
@@ -38,12 +38,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>\log_ab</t>
-  </si>
-  <si>
-    <t>\frac{1}{\log_ab}</t>
-  </si>
-  <si>
     <t>Formula</t>
   </si>
   <si>
@@ -51,6 +45,57 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>20040400105</t>
+  </si>
+  <si>
+    <t>\log_{16}(3x-1)</t>
+  </si>
+  <si>
+    <t>\log_{a}b</t>
+  </si>
+  <si>
+    <t>\frac{1}{\log_{a}b}</t>
+  </si>
+  <si>
+    <t>2\log _{9} x + 1</t>
+  </si>
+  <si>
+    <t>2\log _{x} 3</t>
+  </si>
+  <si>
+    <t>\log_{4}(3x)+\log_{4}(0.5)</t>
+  </si>
+  <si>
+    <t>\log_{2}x-\log_{4}(x-4)</t>
+  </si>
+  <si>
+    <t>20030400103</t>
+  </si>
+  <si>
+    <t>2 + \log_{3}(3x-7)</t>
+  </si>
+  <si>
+    <t>20080400104</t>
+  </si>
+  <si>
+    <t>\log_{3}(2x-3)</t>
+  </si>
+  <si>
+    <t>19980200105</t>
+  </si>
+  <si>
+    <t>\log_{3}(x-1)=2</t>
+  </si>
+  <si>
+    <t>20010400107</t>
+  </si>
+  <si>
+    <t>20020200110</t>
+  </si>
+  <si>
+    <t>\log_{4}y +\log_{2}y</t>
   </si>
 </sst>
 </file>
@@ -366,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -380,7 +425,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -389,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -400,10 +445,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -411,50 +456,114 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>